<commit_message>
EPBDS-6949 Tests for length() and trim()
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" activeTab="7"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="replace" sheetId="14" r:id="rId6"/>
     <sheet name="substring" sheetId="17" r:id="rId7"/>
     <sheet name="concatenate" sheetId="18" r:id="rId8"/>
+    <sheet name="length" sheetId="19" r:id="rId9"/>
+    <sheet name="trim" sheetId="20" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="236">
   <si>
     <t>return contains(str, searchChar);</t>
   </si>
@@ -696,6 +698,39 @@
   </si>
   <si>
     <t>1.55</t>
+  </si>
+  <si>
+    <t>Method int lengthMethod (String str)</t>
+  </si>
+  <si>
+    <t>return length(str);</t>
+  </si>
+  <si>
+    <t>Test lengthMethod lengthTest</t>
+  </si>
+  <si>
+    <t>return trim(str);</t>
+  </si>
+  <si>
+    <t>Test trimMethod trimTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otherwise  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   The rain in Spain stays mainly on the plane   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     text</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Method String trimMethod (String str)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">othe rwise       </t>
   </si>
 </sst>
 </file>
@@ -936,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -993,6 +1028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,29 +1433,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="B3" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1658,25 +1694,25 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="57" t="s">
+      <c r="B35" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -1844,7 +1880,7 @@
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f ca="1">TODAY()</f>
-        <v>43019</v>
+        <v>43024</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>181</v>
@@ -1949,25 +1985,25 @@
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="55" t="s">
+      <c r="B69" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56"/>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="57"/>
-      <c r="D70" s="57"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="58"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="52" t="s">
+      <c r="B72" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="C72" s="53"/>
-      <c r="D72" s="54"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="55"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="5" t="s">
@@ -2184,25 +2220,25 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="55" t="s">
+      <c r="B99" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="C99" s="55"/>
-      <c r="D99" s="55"/>
+      <c r="C99" s="56"/>
+      <c r="D99" s="56"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="58" t="s">
+      <c r="B100" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C100" s="58"/>
-      <c r="D100" s="58"/>
+      <c r="C100" s="59"/>
+      <c r="D100" s="59"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="52" t="s">
+      <c r="B102" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="C102" s="53"/>
-      <c r="D102" s="54"/>
+      <c r="C102" s="54"/>
+      <c r="D102" s="55"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="5" t="s">
@@ -2449,6 +2485,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="56"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="59"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="60"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="48">
+        <v>0</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C14" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D47"/>
@@ -2466,25 +2643,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -2723,25 +2900,25 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
@@ -2891,7 +3068,7 @@
   <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C20"/>
+      <selection activeCell="B2" sqref="B2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2903,22 +3080,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="55"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="59"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -3017,7 +3194,7 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f ca="1">TODAY()</f>
-        <v>43019</v>
+        <v>43024</v>
       </c>
       <c r="C18" s="18" t="b">
         <v>0</v>
@@ -3065,22 +3242,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="55"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="59"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3139,22 +3316,22 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="55"/>
+      <c r="C18" s="56"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="59"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="59"/>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -3242,25 +3419,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3411,25 +3588,25 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
@@ -3575,28 +3752,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3828,31 +4005,31 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="55"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
@@ -4037,25 +4214,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4144,28 +4321,28 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="41" t="s">
@@ -4296,7 +4473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -4309,10 +4486,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="60"/>
+      <c r="C3" s="61"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -4321,11 +4498,11 @@
       <c r="C4" t="s">
         <v>203</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -4477,4 +4654,167 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="56" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="56"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="59"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="60"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <f>LEN(B8)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:C19" si="0">LEN(B9)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="25"/>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="48">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7754 Implement date() and toDate(text, pattern)
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="255">
   <si>
     <t>return contains(str, searchChar);</t>
   </si>
@@ -751,21 +751,6 @@
   </si>
   <si>
     <t>obj</t>
-  </si>
-  <si>
-    <t>return toString(date);</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>07/12/1980</t>
-  </si>
-  <si>
-    <t>Method String dateToStringMethod (Date date)</t>
-  </si>
-  <si>
-    <t>Test dateToStringMethod dateToStringTest</t>
   </si>
   <si>
     <t>Method Integer toIntegerMethod (String str)</t>
@@ -811,9 +796,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1048,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1107,12 +1089,10 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1131,6 +1111,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1140,8 +1123,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1966,7 +1947,7 @@
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f ca="1">TODAY()</f>
-        <v>43050</v>
+        <v>43334</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>181</v>
@@ -2313,11 +2294,11 @@
       <c r="D99" s="61"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="57" t="s">
+      <c r="B100" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C100" s="57"/>
-      <c r="D100" s="57"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="58" t="s">
@@ -2553,11 +2534,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B100:D100"/>
     <mergeCell ref="B102:D102"/>
     <mergeCell ref="B37:D37"/>
@@ -2565,6 +2541,11 @@
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2591,16 +2572,16 @@
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -2714,92 +2695,60 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="61" t="s">
         <v>239</v>
       </c>
       <c r="C2" s="61"/>
-      <c r="E2" s="61" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="61"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+    </row>
+    <row r="3" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="E3" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="F3" s="57"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C3" s="64"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="E6" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="F6" s="66"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C6" s="67"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="41" t="s">
         <v>241</v>
       </c>
       <c r="C7" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="41" t="s">
-        <v>243</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="54">
-        <v>29414</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="30" t="s">
         <v>22</v>
       </c>
@@ -2807,7 +2756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="30" t="s">
         <v>60</v>
       </c>
@@ -2815,7 +2764,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
@@ -2823,7 +2772,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="53">
         <v>0.03</v>
       </c>
@@ -2831,7 +2780,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="33" t="b">
         <v>1</v>
       </c>
@@ -2839,7 +2788,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="48" t="s">
         <v>201</v>
       </c>
@@ -2847,21 +2796,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="55"/>
+      <c r="B24" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E6:F6"/>
+  <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2872,8 +2818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2884,42 +2830,42 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="61" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C3" s="61"/>
       <c r="E3" s="61" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F3" s="61"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="57" t="s">
-        <v>248</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="E4" s="57" t="s">
-        <v>254</v>
-      </c>
-      <c r="F4" s="57"/>
+      <c r="B4" s="64" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" s="64"/>
+      <c r="E4" s="64" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="64"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" s="66"/>
+        <v>244</v>
+      </c>
+      <c r="C7" s="67"/>
       <c r="E7" s="58" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="66"/>
+        <v>250</v>
+      </c>
+      <c r="F7" s="67"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="56" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="56" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="43" t="s">
@@ -2956,13 +2902,13 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="26" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F11" s="2">
         <v>1.3</v>
@@ -2970,13 +2916,13 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="26" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C12" s="2">
         <v>-1</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F12" s="2">
         <v>-1</v>
@@ -2984,27 +2930,27 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C13" s="2">
         <v>1234567890</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F13" s="2">
         <v>1234.56789</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="68" t="s">
-        <v>258</v>
+      <c r="B14" s="57" t="s">
+        <v>253</v>
       </c>
       <c r="C14" s="45">
         <v>12</v>
       </c>
-      <c r="E14" s="68" t="s">
-        <v>259</v>
+      <c r="E14" s="57" t="s">
+        <v>254</v>
       </c>
       <c r="F14" s="45">
         <v>1.1000000000000001</v>
@@ -3048,11 +2994,11 @@
       <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="58" t="s">
@@ -3305,11 +3251,11 @@
       <c r="D32" s="61"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="57" t="s">
+      <c r="B33" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="58" t="s">
@@ -3484,16 +3430,16 @@
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -3592,7 +3538,7 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f ca="1">TODAY()</f>
-        <v>43050</v>
+        <v>43334</v>
       </c>
       <c r="C18" s="18" t="b">
         <v>0</v>
@@ -3646,16 +3592,16 @@
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3720,16 +3666,16 @@
       <c r="C18" s="61"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="57"/>
+      <c r="C19" s="64"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="64"/>
+      <c r="C21" s="65"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -3824,11 +3770,11 @@
       <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="58" t="s">
@@ -3993,11 +3939,11 @@
       <c r="D26" s="61"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="58" t="s">
@@ -4158,12 +4104,12 @@
       <c r="E2" s="61"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="58" t="s">
@@ -4412,13 +4358,13 @@
       <c r="F29" s="61"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="58" t="s">
@@ -4619,11 +4565,11 @@
       <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="58" t="s">
@@ -4727,12 +4673,12 @@
       <c r="E19" s="61"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="58" t="s">
@@ -4884,10 +4830,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="66" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="65"/>
+      <c r="C3" s="66"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -4896,11 +4842,11 @@
       <c r="C4" t="s">
         <v>203</v>
       </c>
-      <c r="F4" s="65" t="s">
+      <c r="F4" s="66" t="s">
         <v>219</v>
       </c>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -5074,16 +5020,16 @@
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">

</xml_diff>

<commit_message>
EPBDS-7884 implemented isInteger() isNumber() isDate() functions
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" activeTab="10"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -19,13 +24,16 @@
     <sheet name="trim" sheetId="20" r:id="rId10"/>
     <sheet name="toString" sheetId="21" r:id="rId11"/>
     <sheet name="toNumbers" sheetId="22" r:id="rId12"/>
+    <sheet name="isInteger" sheetId="23" r:id="rId13"/>
+    <sheet name="IsNumber" sheetId="24" r:id="rId14"/>
+    <sheet name="isDate" sheetId="25" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="382">
   <si>
     <t>return contains(str, searchChar);</t>
   </si>
@@ -790,12 +798,393 @@
   </si>
   <si>
     <t>0001.10000</t>
+  </si>
+  <si>
+    <t>return isInteger(str);</t>
+  </si>
+  <si>
+    <t>return isInteger(new Object());</t>
+  </si>
+  <si>
+    <t>return isInteger(i);</t>
+  </si>
+  <si>
+    <t>Test isIntegerMethod</t>
+  </si>
+  <si>
+    <t>_description_</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>123-</t>
+  </si>
+  <si>
+    <t>123+</t>
+  </si>
+  <si>
+    <t>12+34</t>
+  </si>
+  <si>
+    <t>12,34</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>123d</t>
+  </si>
+  <si>
+    <t>12 34</t>
+  </si>
+  <si>
+    <t>12a34</t>
+  </si>
+  <si>
+    <t>a1234</t>
+  </si>
+  <si>
+    <t>1234b</t>
+  </si>
+  <si>
+    <t>1234l</t>
+  </si>
+  <si>
+    <t>1234L</t>
+  </si>
+  <si>
+    <t>12-34</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>.123</t>
+  </si>
+  <si>
+    <t>+.123</t>
+  </si>
+  <si>
+    <t>-.123</t>
+  </si>
+  <si>
+    <t>++123</t>
+  </si>
+  <si>
+    <t>--123</t>
+  </si>
+  <si>
+    <t>-+123</t>
+  </si>
+  <si>
+    <t>+1234</t>
+  </si>
+  <si>
+    <t>-1234</t>
+  </si>
+  <si>
+    <t>+0</t>
+  </si>
+  <si>
+    <t>-0</t>
+  </si>
+  <si>
+    <t>Test isIntegerWhenObjectPassed</t>
+  </si>
+  <si>
+    <t>Test isIntegerWhenIntegerPassed</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Method boolean isIntegerMethod(String str)</t>
+  </si>
+  <si>
+    <t>Method boolean isIntegerWhenObjectPassed()</t>
+  </si>
+  <si>
+    <t>Method boolean isIntegerWhenIntegerPassed(Integer i)</t>
+  </si>
+  <si>
+    <t>Method boolean isIntegerWhenDoublePassed(Double i)</t>
+  </si>
+  <si>
+    <t>Test isIntegerWhenDoublePassed</t>
+  </si>
+  <si>
+    <t>Method boolean isIntegerWhenLongPassed(Long i)</t>
+  </si>
+  <si>
+    <t>Test  isIntegerWhenLongPassed</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>return isNumber(new Object());</t>
+  </si>
+  <si>
+    <t>return isNumber(i);</t>
+  </si>
+  <si>
+    <t>Test isNumberMethod</t>
+  </si>
+  <si>
+    <t>Test isNumberWhenObjectPassed</t>
+  </si>
+  <si>
+    <t>Test isNumberWhenIntegerPassed</t>
+  </si>
+  <si>
+    <t>Test isNumberWhenDoublePassed</t>
+  </si>
+  <si>
+    <t>Method boolean isNumberWhenLongPassed(Long i)</t>
+  </si>
+  <si>
+    <t>Test  isNumberWhenLongPassed</t>
+  </si>
+  <si>
+    <t>Method boolean isNumberMethod(String str)</t>
+  </si>
+  <si>
+    <t>Method boolean isNumberWhenObjectPassed()</t>
+  </si>
+  <si>
+    <t>Method boolean isNumberWhenIntegerPassed(Integer i)</t>
+  </si>
+  <si>
+    <t>Method boolean isNumberWhenDoublePassed(Double i)</t>
+  </si>
+  <si>
+    <t>return isNumber(str);</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>NAN</t>
+  </si>
+  <si>
+    <t>nAn</t>
+  </si>
+  <si>
+    <t>naN</t>
+  </si>
+  <si>
+    <t>NaN1</t>
+  </si>
+  <si>
+    <t>1NaN</t>
+  </si>
+  <si>
+    <t>-NaN-</t>
+  </si>
+  <si>
+    <t>NaN+</t>
+  </si>
+  <si>
+    <t>NaN-</t>
+  </si>
+  <si>
+    <t>1.23.4</t>
+  </si>
+  <si>
+    <t>123.3E1.</t>
+  </si>
+  <si>
+    <t>123.3E</t>
+  </si>
+  <si>
+    <t>123.3E1E1</t>
+  </si>
+  <si>
+    <t>123.+E1</t>
+  </si>
+  <si>
+    <t>123.-E1</t>
+  </si>
+  <si>
+    <t>123.3ED</t>
+  </si>
+  <si>
+    <t>123.3E-D</t>
+  </si>
+  <si>
+    <t>123.3E+F</t>
+  </si>
+  <si>
+    <t>+000E.123</t>
+  </si>
+  <si>
+    <t>-000E.123</t>
+  </si>
+  <si>
+    <t>123E4l</t>
+  </si>
+  <si>
+    <t>.E21</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>+NaN</t>
+  </si>
+  <si>
+    <t>-NaN</t>
+  </si>
+  <si>
+    <t>123D</t>
+  </si>
+  <si>
+    <t>123f</t>
+  </si>
+  <si>
+    <t>123F</t>
+  </si>
+  <si>
+    <t>123.F</t>
+  </si>
+  <si>
+    <t>123.4E21</t>
+  </si>
+  <si>
+    <t>123.E21</t>
+  </si>
+  <si>
+    <t>123.E21F</t>
+  </si>
+  <si>
+    <t>123.E21D</t>
+  </si>
+  <si>
+    <t>1234E5</t>
+  </si>
+  <si>
+    <t>1234E+5</t>
+  </si>
+  <si>
+    <t>1234E-5</t>
+  </si>
+  <si>
+    <t>-0001.123</t>
+  </si>
+  <si>
+    <t>-000.123</t>
+  </si>
+  <si>
+    <t>+00.123</t>
+  </si>
+  <si>
+    <t>+0002.123</t>
+  </si>
+  <si>
+    <t>Method boolean isDateMethod(String str)</t>
+  </si>
+  <si>
+    <t>return isDate(str);</t>
+  </si>
+  <si>
+    <t>return isDate(str, pattern);</t>
+  </si>
+  <si>
+    <t>Method boolean isDateWithPatternMethod(String str, String pattern)</t>
+  </si>
+  <si>
+    <t>Test isDateMethod</t>
+  </si>
+  <si>
+    <t>12.30</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>2014-12-12</t>
+  </si>
+  <si>
+    <t>06.27.2014</t>
+  </si>
+  <si>
+    <t>06/17/2014</t>
+  </si>
+  <si>
+    <t>31/17/2014</t>
+  </si>
+  <si>
+    <t>Test isDateWithPatternMethod</t>
+  </si>
+  <si>
+    <t>yyy-dd-MM</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t>2014-13-12</t>
+  </si>
+  <si>
+    <t>MM.dd.yyyy</t>
+  </si>
+  <si>
+    <t>oo.oo.2014</t>
+  </si>
+  <si>
+    <t>06/27.2014</t>
+  </si>
+  <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Method boolean isDateMethodWhenDate(Date date)</t>
+  </si>
+  <si>
+    <t>return isDate(date);</t>
+  </si>
+  <si>
+    <t>Test isDateMethodWhenDate</t>
+  </si>
+  <si>
+    <t>Method boolean isDateMethodWhenObject()</t>
+  </si>
+  <si>
+    <t>return isDate(new Object());</t>
+  </si>
+  <si>
+    <t>Test isDateMethodWhenObject</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1030,7 +1419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1093,6 +1482,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1111,9 +1505,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,13 +1516,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1500,29 +1894,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="B3" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1761,25 +2155,25 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="60"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="63"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -1947,7 +2341,7 @@
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f ca="1">TODAY()</f>
-        <v>43334</v>
+        <v>43397</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>181</v>
@@ -2052,25 +2446,25 @@
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="61" t="s">
+      <c r="B69" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
+      <c r="C69" s="65"/>
+      <c r="D69" s="65"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="63" t="s">
+      <c r="B70" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="63"/>
-      <c r="D70" s="63"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="C72" s="59"/>
-      <c r="D72" s="60"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="63"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="5" t="s">
@@ -2287,25 +2681,25 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="61" t="s">
+      <c r="B99" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="C99" s="61"/>
-      <c r="D99" s="61"/>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="64" t="s">
+      <c r="B100" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="C100" s="64"/>
-      <c r="D100" s="64"/>
+      <c r="C100" s="60"/>
+      <c r="D100" s="60"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="58" t="s">
+      <c r="B102" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="C102" s="59"/>
-      <c r="D102" s="60"/>
+      <c r="C102" s="62"/>
+      <c r="D102" s="63"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="5" t="s">
@@ -2534,6 +2928,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B100:D100"/>
     <mergeCell ref="B102:D102"/>
     <mergeCell ref="B37:D37"/>
@@ -2541,11 +2940,6 @@
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2566,22 +2960,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="64"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>229</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -2697,7 +3091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -2707,22 +3101,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="64"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="61" t="s">
         <v>240</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="41" t="s">
@@ -2829,34 +3223,34 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="E3" s="61" t="s">
+      <c r="C3" s="64"/>
+      <c r="E3" s="64" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="61"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="60" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="E4" s="64" t="s">
+      <c r="C4" s="60"/>
+      <c r="E4" s="60" t="s">
         <v>249</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="61" t="s">
         <v>244</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="E7" s="58" t="s">
+      <c r="C7" s="69"/>
+      <c r="E7" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="F7" s="67"/>
+      <c r="F7" s="69"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="56" t="s">
@@ -2967,6 +3361,2742 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:V112"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:V38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B3" s="68" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="G3" s="68" t="s">
+        <v>294</v>
+      </c>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="L3" s="68" t="s">
+        <v>295</v>
+      </c>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="R3" s="68" t="s">
+        <v>296</v>
+      </c>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B4" s="68" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="G4" s="68" t="s">
+        <v>256</v>
+      </c>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="L4" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="R4" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B7" s="68" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="G7" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="L7" s="68" t="s">
+        <v>289</v>
+      </c>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="R7" s="68" t="s">
+        <v>297</v>
+      </c>
+      <c r="S7" s="68"/>
+      <c r="T7" s="68"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>259</v>
+      </c>
+      <c r="M8" t="s">
+        <v>290</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" t="s">
+        <v>259</v>
+      </c>
+      <c r="S8" t="s">
+        <v>290</v>
+      </c>
+      <c r="T8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>260</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>260</v>
+      </c>
+      <c r="M9" t="s">
+        <v>291</v>
+      </c>
+      <c r="N9" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
+        <v>260</v>
+      </c>
+      <c r="S9" t="s">
+        <v>292</v>
+      </c>
+      <c r="T9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H10" t="s">
+        <v>262</v>
+      </c>
+      <c r="L10" t="s">
+        <v>60</v>
+      </c>
+      <c r="N10" t="s">
+        <v>262</v>
+      </c>
+      <c r="R10" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C11" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
+        <v>262</v>
+      </c>
+      <c r="M11">
+        <v>123</v>
+      </c>
+      <c r="N11" t="s">
+        <v>238</v>
+      </c>
+      <c r="S11">
+        <v>1.23</v>
+      </c>
+      <c r="T11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C12" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C13" s="47" t="s">
+        <v>264</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C14" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C15" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C16" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="D16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" s="68" t="s">
+        <v>298</v>
+      </c>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+      <c r="G17" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="D18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C19" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" t="s">
+        <v>262</v>
+      </c>
+      <c r="G20" s="68" t="s">
+        <v>299</v>
+      </c>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" t="s">
+        <v>259</v>
+      </c>
+      <c r="H21" t="s">
+        <v>290</v>
+      </c>
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+      <c r="G22" t="s">
+        <v>260</v>
+      </c>
+      <c r="H22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" t="s">
+        <v>262</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D24" t="s">
+        <v>262</v>
+      </c>
+      <c r="H24">
+        <v>123</v>
+      </c>
+      <c r="I24" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C25" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C26" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="D26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C27" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C28" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C29" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="D29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C30" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C31" s="47" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C32" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="D34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="D35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="D37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="47"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="47"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="47"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C43" s="47"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C44" s="47"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C45" s="47"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C46" s="47"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="47"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="47"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="47"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="47"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="47"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="47"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="47"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="47"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="47"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="47"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="47"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="47"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="47"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="47"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="47"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="47"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="47"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="47"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="47"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="47"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="47"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="47"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="47"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="47"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="47"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="47"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="47"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="47"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="47"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="47"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="47"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="47"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="47"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="47"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="47"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="47"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="47"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" s="47"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" s="47"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" s="47"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" s="47"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" s="47"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" s="47"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" s="47"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" s="47"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92" s="47"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C93" s="47"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C94" s="47"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C95" s="47"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C96" s="47"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C97" s="47"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C98" s="47"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" s="47"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="47"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" s="47"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" s="47"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C103" s="47"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C104" s="47"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C105" s="47"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C106" s="47"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C107" s="47"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C108" s="47"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C109" s="47"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C110" s="47"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C111" s="47"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C112" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="R3:V3"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="L4:P4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:V344"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B2" s="68" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="G2" s="68" t="s">
+        <v>310</v>
+      </c>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="L2" s="68" t="s">
+        <v>311</v>
+      </c>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="R2" s="68" t="s">
+        <v>312</v>
+      </c>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68"/>
+      <c r="V2" s="68"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B3" s="68" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="G3" s="68" t="s">
+        <v>301</v>
+      </c>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="L3" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="R3" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B6" s="68" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="G6" s="58" t="s">
+        <v>304</v>
+      </c>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="L6" s="68" t="s">
+        <v>305</v>
+      </c>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="R6" s="68" t="s">
+        <v>306</v>
+      </c>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>259</v>
+      </c>
+      <c r="M7" t="s">
+        <v>290</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>259</v>
+      </c>
+      <c r="S7" t="s">
+        <v>290</v>
+      </c>
+      <c r="T7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>260</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>260</v>
+      </c>
+      <c r="M8" t="s">
+        <v>291</v>
+      </c>
+      <c r="N8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" t="s">
+        <v>260</v>
+      </c>
+      <c r="S8" t="s">
+        <v>292</v>
+      </c>
+      <c r="T8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" t="s">
+        <v>262</v>
+      </c>
+      <c r="H9" t="s">
+        <v>262</v>
+      </c>
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>262</v>
+      </c>
+      <c r="R9" t="s">
+        <v>60</v>
+      </c>
+      <c r="T9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C10" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" t="s">
+        <v>262</v>
+      </c>
+      <c r="M10">
+        <v>123</v>
+      </c>
+      <c r="N10" t="s">
+        <v>238</v>
+      </c>
+      <c r="S10">
+        <v>1.23</v>
+      </c>
+      <c r="T10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C11" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C12" s="47" t="s">
+        <v>314</v>
+      </c>
+      <c r="D12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C13" s="47" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C14" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C15" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="D15" t="s">
+        <v>262</v>
+      </c>
+      <c r="G15" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="C16" s="47" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C17" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="D18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="D19" t="s">
+        <v>262</v>
+      </c>
+      <c r="G19" s="68" t="s">
+        <v>308</v>
+      </c>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="D20" t="s">
+        <v>262</v>
+      </c>
+      <c r="G20" t="s">
+        <v>259</v>
+      </c>
+      <c r="H20" t="s">
+        <v>290</v>
+      </c>
+      <c r="I20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C21" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" t="s">
+        <v>260</v>
+      </c>
+      <c r="H21" t="s">
+        <v>300</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" t="s">
+        <v>262</v>
+      </c>
+      <c r="H23">
+        <v>123</v>
+      </c>
+      <c r="I23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="D27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D28" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="47" t="s">
+        <v>318</v>
+      </c>
+      <c r="D29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="47" t="s">
+        <v>319</v>
+      </c>
+      <c r="D30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C31" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="D32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="D33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="D34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="47" t="s">
+        <v>324</v>
+      </c>
+      <c r="D35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="47" t="s">
+        <v>325</v>
+      </c>
+      <c r="D36" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="47" t="s">
+        <v>326</v>
+      </c>
+      <c r="D37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="D38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="D39" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="47" t="s">
+        <v>329</v>
+      </c>
+      <c r="D40" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="47" t="s">
+        <v>330</v>
+      </c>
+      <c r="D41" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="47" t="s">
+        <v>331</v>
+      </c>
+      <c r="D42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C43" s="47" t="s">
+        <v>332</v>
+      </c>
+      <c r="D43" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C44" s="47" t="s">
+        <v>333</v>
+      </c>
+      <c r="D44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C45" s="47" t="s">
+        <v>334</v>
+      </c>
+      <c r="D45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C46" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="D46" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="47" t="s">
+        <v>336</v>
+      </c>
+      <c r="D47" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="47" t="s">
+        <v>337</v>
+      </c>
+      <c r="D48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="D49" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="47" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D51" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="D52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="D53" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="D54" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="47" t="s">
+        <v>339</v>
+      </c>
+      <c r="D55" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="47" t="s">
+        <v>340</v>
+      </c>
+      <c r="D56" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="D57" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="D58" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="D62" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C63" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="D63" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C64" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="D64" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="D65" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="D66" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="D67" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C68" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D68" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D69" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C70" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="D70" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="47" t="s">
+        <v>346</v>
+      </c>
+      <c r="D71" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C72" s="47" t="s">
+        <v>347</v>
+      </c>
+      <c r="D72" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="47" t="s">
+        <v>348</v>
+      </c>
+      <c r="D73" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="47" t="s">
+        <v>349</v>
+      </c>
+      <c r="D74" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="47" t="s">
+        <v>350</v>
+      </c>
+      <c r="D75" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C76" s="47" t="s">
+        <v>351</v>
+      </c>
+      <c r="D76" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C77" s="47" t="s">
+        <v>352</v>
+      </c>
+      <c r="D77" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="47" t="s">
+        <v>353</v>
+      </c>
+      <c r="D78" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="47"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C80" s="47"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="47"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="47"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="47"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" s="47"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" s="47"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" s="47"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" s="47"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" s="47"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" s="47"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" s="47"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" s="47"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92" s="47"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C93" s="47"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C94" s="47"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C95" s="47"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C96" s="47"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C97" s="47"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C98" s="47"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" s="47"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="47"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" s="47"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" s="47"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C103" s="47"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C104" s="47"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C105" s="47"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C106" s="47"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C107" s="47"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C108" s="47"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C109" s="47"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C110" s="47"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C111" s="47"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C112" s="47"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C113" s="47"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C114" s="47"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C115" s="47"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C116" s="47"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C117" s="47"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C118" s="47"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C119" s="47"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C120" s="47"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C121" s="47"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C122" s="47"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C123" s="47"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C124" s="47"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C125" s="47"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C126" s="47"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C127" s="47"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C128" s="47"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C129" s="47"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C130" s="47"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C131" s="47"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C132" s="47"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C133" s="47"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C134" s="47"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C135" s="47"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C136" s="47"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C137" s="47"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C138" s="47"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C139" s="47"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C140" s="47"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C141" s="47"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C142" s="47"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C143" s="47"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C144" s="47"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C145" s="47"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C146" s="47"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C147" s="47"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C148" s="47"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C149" s="47"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C150" s="47"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C151" s="47"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C152" s="47"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C153" s="47"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C154" s="47"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C155" s="47"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C156" s="47"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C157" s="47"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C158" s="47"/>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C159" s="47"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C160" s="47"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C161" s="47"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C162" s="47"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C163" s="47"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C164" s="47"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C165" s="47"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C166" s="47"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C167" s="47"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C168" s="47"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C169" s="47"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C170" s="47"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C171" s="47"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C172" s="47"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C173" s="47"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C174" s="47"/>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C175" s="47"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C176" s="47"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C177" s="47"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C178" s="47"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C179" s="47"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C180" s="47"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C181" s="47"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C182" s="47"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C183" s="47"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C184" s="47"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C185" s="47"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C186" s="47"/>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C187" s="47"/>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C188" s="47"/>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C189" s="47"/>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C190" s="47"/>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C191" s="47"/>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C192" s="47"/>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C193" s="47"/>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C194" s="47"/>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C195" s="47"/>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C196" s="47"/>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C197" s="47"/>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C198" s="47"/>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C199" s="47"/>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C200" s="47"/>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C201" s="47"/>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C202" s="47"/>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C203" s="47"/>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C204" s="47"/>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C205" s="47"/>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C206" s="47"/>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C207" s="47"/>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C208" s="47"/>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C209" s="47"/>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C210" s="47"/>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C211" s="47"/>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C212" s="47"/>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C213" s="47"/>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C214" s="47"/>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C215" s="47"/>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C216" s="47"/>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C217" s="47"/>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C218" s="47"/>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C219" s="47"/>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C220" s="47"/>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C221" s="47"/>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C222" s="47"/>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C223" s="47"/>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C224" s="47"/>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C225" s="47"/>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C226" s="47"/>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C227" s="47"/>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C228" s="47"/>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C229" s="47"/>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C230" s="47"/>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C231" s="47"/>
+    </row>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C232" s="47"/>
+    </row>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C233" s="47"/>
+    </row>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C234" s="47"/>
+    </row>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C235" s="47"/>
+    </row>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C236" s="47"/>
+    </row>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C237" s="47"/>
+    </row>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C238" s="47"/>
+    </row>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C239" s="47"/>
+    </row>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C240" s="47"/>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C241" s="47"/>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C242" s="47"/>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C243" s="47"/>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C244" s="47"/>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C245" s="47"/>
+    </row>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C246" s="47"/>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C247" s="47"/>
+    </row>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C248" s="47"/>
+    </row>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C249" s="47"/>
+    </row>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C250" s="47"/>
+    </row>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C251" s="47"/>
+    </row>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C252" s="47"/>
+    </row>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C253" s="47"/>
+    </row>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C254" s="47"/>
+    </row>
+    <row r="255" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C255" s="47"/>
+    </row>
+    <row r="256" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C256" s="47"/>
+    </row>
+    <row r="257" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C257" s="47"/>
+    </row>
+    <row r="258" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C258" s="47"/>
+    </row>
+    <row r="259" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C259" s="47"/>
+    </row>
+    <row r="260" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C260" s="47"/>
+    </row>
+    <row r="261" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C261" s="47"/>
+    </row>
+    <row r="262" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C262" s="47"/>
+    </row>
+    <row r="263" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C263" s="47"/>
+    </row>
+    <row r="264" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C264" s="47"/>
+    </row>
+    <row r="265" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C265" s="47"/>
+    </row>
+    <row r="266" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C266" s="47"/>
+    </row>
+    <row r="267" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C267" s="47"/>
+    </row>
+    <row r="268" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C268" s="47"/>
+    </row>
+    <row r="269" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C269" s="47"/>
+    </row>
+    <row r="270" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C270" s="47"/>
+    </row>
+    <row r="271" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C271" s="47"/>
+    </row>
+    <row r="272" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C272" s="47"/>
+    </row>
+    <row r="273" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C273" s="47"/>
+    </row>
+    <row r="274" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C274" s="47"/>
+    </row>
+    <row r="275" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C275" s="47"/>
+    </row>
+    <row r="276" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C276" s="47"/>
+    </row>
+    <row r="277" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C277" s="47"/>
+    </row>
+    <row r="278" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C278" s="47"/>
+    </row>
+    <row r="279" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C279" s="47"/>
+    </row>
+    <row r="280" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C280" s="47"/>
+    </row>
+    <row r="281" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C281" s="47"/>
+    </row>
+    <row r="282" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C282" s="47"/>
+    </row>
+    <row r="283" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C283" s="47"/>
+    </row>
+    <row r="284" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C284" s="47"/>
+    </row>
+    <row r="285" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C285" s="47"/>
+    </row>
+    <row r="286" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C286" s="47"/>
+    </row>
+    <row r="287" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C287" s="47"/>
+    </row>
+    <row r="288" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C288" s="47"/>
+    </row>
+    <row r="289" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C289" s="47"/>
+    </row>
+    <row r="290" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C290" s="47"/>
+    </row>
+    <row r="291" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C291" s="47"/>
+    </row>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C292" s="47"/>
+    </row>
+    <row r="293" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C293" s="47"/>
+    </row>
+    <row r="294" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C294" s="47"/>
+    </row>
+    <row r="295" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C295" s="47"/>
+    </row>
+    <row r="296" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C296" s="47"/>
+    </row>
+    <row r="297" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C297" s="47"/>
+    </row>
+    <row r="298" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C298" s="47"/>
+    </row>
+    <row r="299" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C299" s="47"/>
+    </row>
+    <row r="300" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C300" s="47"/>
+    </row>
+    <row r="301" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C301" s="47"/>
+    </row>
+    <row r="302" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C302" s="47"/>
+    </row>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C303" s="47"/>
+    </row>
+    <row r="304" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C304" s="47"/>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C305" s="47"/>
+    </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C306" s="47"/>
+    </row>
+    <row r="307" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C307" s="47"/>
+    </row>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C308" s="47"/>
+    </row>
+    <row r="309" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C309" s="47"/>
+    </row>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C310" s="47"/>
+    </row>
+    <row r="311" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C311" s="47"/>
+    </row>
+    <row r="312" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C312" s="47"/>
+    </row>
+    <row r="313" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C313" s="47"/>
+    </row>
+    <row r="314" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C314" s="47"/>
+    </row>
+    <row r="315" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C315" s="47"/>
+    </row>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C316" s="47"/>
+    </row>
+    <row r="317" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C317" s="47"/>
+    </row>
+    <row r="318" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C318" s="47"/>
+    </row>
+    <row r="319" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C319" s="47"/>
+    </row>
+    <row r="320" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C320" s="47"/>
+    </row>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C321" s="47"/>
+    </row>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C322" s="47"/>
+    </row>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C323" s="47"/>
+    </row>
+    <row r="324" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C324" s="47"/>
+    </row>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C325" s="47"/>
+    </row>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C326" s="47"/>
+    </row>
+    <row r="327" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C327" s="47"/>
+    </row>
+    <row r="328" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C328" s="47"/>
+    </row>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C329" s="47"/>
+    </row>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C330" s="47"/>
+    </row>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C331" s="47"/>
+    </row>
+    <row r="332" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C332" s="47"/>
+    </row>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C333" s="47"/>
+    </row>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C334" s="47"/>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C335" s="47"/>
+    </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C336" s="47"/>
+    </row>
+    <row r="337" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C337" s="47"/>
+    </row>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C338" s="47"/>
+    </row>
+    <row r="339" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C339" s="47"/>
+    </row>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C340" s="47"/>
+    </row>
+    <row r="341" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C341" s="47"/>
+    </row>
+    <row r="342" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C342" s="47"/>
+    </row>
+    <row r="343" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C343" s="47"/>
+    </row>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C344" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="R3:V3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Y38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B2" s="68" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="G2" s="68" t="s">
+        <v>357</v>
+      </c>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="O2" s="68" t="s">
+        <v>374</v>
+      </c>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="U2" s="68" t="s">
+        <v>377</v>
+      </c>
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="68"/>
+      <c r="Y2" s="68"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="G3" s="68" t="s">
+        <v>356</v>
+      </c>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="O3" s="68" t="s">
+        <v>375</v>
+      </c>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="U3" s="68" t="s">
+        <v>378</v>
+      </c>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="G6" s="68" t="s">
+        <v>365</v>
+      </c>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="O6" s="68" t="s">
+        <v>376</v>
+      </c>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="58"/>
+      <c r="U6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B7" s="68" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="G7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>372</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>259</v>
+      </c>
+      <c r="P7" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>260</v>
+      </c>
+      <c r="H8" t="s">
+        <v>261</v>
+      </c>
+      <c r="I8" t="s">
+        <v>373</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" t="s">
+        <v>260</v>
+      </c>
+      <c r="P8" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="47"/>
+      <c r="J9" t="s">
+        <v>262</v>
+      </c>
+      <c r="O9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P9" s="47"/>
+      <c r="Q9" t="s">
+        <v>262</v>
+      </c>
+      <c r="U9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="J10" t="s">
+        <v>238</v>
+      </c>
+      <c r="P10" s="59">
+        <v>41255</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C11" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" t="s">
+        <v>262</v>
+      </c>
+      <c r="H11" s="47"/>
+      <c r="I11" t="s">
+        <v>366</v>
+      </c>
+      <c r="J11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C12" s="47" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="I12" t="s">
+        <v>367</v>
+      </c>
+      <c r="J12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C13" s="47" t="s">
+        <v>360</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="I13" t="s">
+        <v>367</v>
+      </c>
+      <c r="J13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C14" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="D14" t="s">
+        <v>262</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="I14" t="s">
+        <v>369</v>
+      </c>
+      <c r="J14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C15" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="D15" t="s">
+        <v>262</v>
+      </c>
+      <c r="H15" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="I15" t="s">
+        <v>369</v>
+      </c>
+      <c r="J15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C16" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="D16" t="s">
+        <v>238</v>
+      </c>
+      <c r="H16" s="47" t="s">
+        <v>371</v>
+      </c>
+      <c r="I16" t="s">
+        <v>369</v>
+      </c>
+      <c r="J16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+      <c r="H17" s="47"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="47"/>
+      <c r="H18" s="47"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="47"/>
+      <c r="H19" s="47"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="47"/>
+      <c r="H20" s="47"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="47"/>
+      <c r="H21" s="47"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="47"/>
+      <c r="H22" s="47"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="47"/>
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="47"/>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="47"/>
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="47"/>
+      <c r="H26" s="47"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C27" s="47"/>
+      <c r="H27" s="47"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="47"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C29" s="47"/>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="47"/>
+      <c r="H30" s="47"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C31" s="47"/>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="47"/>
+      <c r="H32" s="47"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="47"/>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="47"/>
+      <c r="H34" s="47"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="47"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="47"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="47"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="G3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2987,25 +6117,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3244,25 +6374,25 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="63"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
@@ -3424,22 +6554,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="64"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -3538,7 +6668,7 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f ca="1">TODAY()</f>
-        <v>43334</v>
+        <v>43397</v>
       </c>
       <c r="C18" s="18" t="b">
         <v>0</v>
@@ -3586,22 +6716,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="64"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3660,22 +6790,22 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="64"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="64"/>
+      <c r="C19" s="60"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="67" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="65"/>
+      <c r="C21" s="67"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -3763,25 +6893,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3932,25 +7062,25 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="63"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
@@ -4096,28 +7226,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4349,31 +7479,31 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="63"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
@@ -4558,25 +7688,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4665,28 +7795,28 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="63"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="41" t="s">
@@ -4830,10 +7960,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="68" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="66"/>
+      <c r="C3" s="68"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -4842,11 +7972,11 @@
       <c r="C4" t="s">
         <v>203</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="F4" s="68" t="s">
         <v>219</v>
       </c>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -5014,22 +8144,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="64"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">

</xml_diff>

<commit_message>
EPBDS-7884 implemented like function
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="3" activeTab="14"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="4" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="isInteger" sheetId="23" r:id="rId13"/>
     <sheet name="IsNumber" sheetId="24" r:id="rId14"/>
     <sheet name="isDate" sheetId="25" r:id="rId15"/>
+    <sheet name="like" sheetId="26" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="422">
   <si>
     <t>return contains(str, searchChar);</t>
   </si>
@@ -1179,6 +1180,126 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Method boolean likeMethod(String str, String pattern)</t>
+  </si>
+  <si>
+    <t>return like(str, pattern);</t>
+  </si>
+  <si>
+    <t>Test likeMethod</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>FFF</t>
+  </si>
+  <si>
+    <t>[!A-Z]</t>
+  </si>
+  <si>
+    <t>aTa</t>
+  </si>
+  <si>
+    <t>a#a</t>
+  </si>
+  <si>
+    <t>CAT123khg</t>
+  </si>
+  <si>
+    <t>B?T*</t>
+  </si>
+  <si>
+    <t>a2a</t>
+  </si>
+  <si>
+    <t>a@a</t>
+  </si>
+  <si>
+    <t>1E1234AE</t>
+  </si>
+  <si>
+    <t>@@####@@</t>
+  </si>
+  <si>
+    <t>A23-45AE</t>
+  </si>
+  <si>
+    <t>###-##@@</t>
+  </si>
+  <si>
+    <t>foo.bar@gmail.</t>
+  </si>
+  <si>
+    <t>foo.bar@gmailcom</t>
+  </si>
+  <si>
+    <t>+38(099)123-12-12</t>
+  </si>
+  <si>
+    <t>+7#(###)###-##-##</t>
+  </si>
+  <si>
+    <t>aBBBa</t>
+  </si>
+  <si>
+    <t>a*a</t>
+  </si>
+  <si>
+    <t>[A-Z]</t>
+  </si>
+  <si>
+    <t>BAR+</t>
+  </si>
+  <si>
+    <t>[A-Z]++</t>
+  </si>
+  <si>
+    <t>aM5b</t>
+  </si>
+  <si>
+    <t>a[L-P]#[!c-e]</t>
+  </si>
+  <si>
+    <t>BAT123khg</t>
+  </si>
+  <si>
+    <t>AE1234AE</t>
+  </si>
+  <si>
+    <t>123-45AE</t>
+  </si>
+  <si>
+    <t>###-##??+</t>
+  </si>
+  <si>
+    <t>123-45AE123</t>
+  </si>
+  <si>
+    <t>123-45-AE</t>
+  </si>
+  <si>
+    <t>#+-#+-@+</t>
+  </si>
+  <si>
+    <t>foo.bar@gmail.com</t>
+  </si>
+  <si>
+    <t>foo@bar.com</t>
+  </si>
+  <si>
+    <t>+38(099) 123-12-12</t>
+  </si>
+  <si>
+    <t>+##(###) ###-##-##</t>
+  </si>
+  <si>
+    <t>?+\@?+.?+</t>
+  </si>
+  <si>
+    <t>*\@*.*</t>
   </si>
 </sst>
 </file>
@@ -5687,7 +5808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
@@ -6095,6 +6216,490 @@
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="68" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="68" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="47"/>
+      <c r="D12" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="E12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="E14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="E15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="47" t="s">
+        <v>388</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>389</v>
+      </c>
+      <c r="E16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="47" t="s">
+        <v>390</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="E17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="47" t="s">
+        <v>392</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="E18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="E19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="E20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21" s="47" t="s">
+        <v>398</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="E21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" s="47" t="s">
+        <v>399</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="E22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="47" t="s">
+        <v>400</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>401</v>
+      </c>
+      <c r="E23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="47" t="s">
+        <v>402</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>403</v>
+      </c>
+      <c r="E25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>404</v>
+      </c>
+      <c r="E26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C27" s="47" t="s">
+        <v>405</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="E27" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="47" t="s">
+        <v>392</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>389</v>
+      </c>
+      <c r="E28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C29" s="47" t="s">
+        <v>388</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="E29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C30" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>408</v>
+      </c>
+      <c r="E30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="E31" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C32" s="47" t="s">
+        <v>410</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="E32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="E33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="E34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="E35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="47" t="s">
+        <v>413</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="E36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="D37" s="47" t="s">
+        <v>415</v>
+      </c>
+      <c r="E37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="47" t="s">
+        <v>416</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="E38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="D39" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="E39" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="E40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPDBS-7884 use US locale by default
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="4" activeTab="15"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -5808,8 +5808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.2">
       <c r="C15" s="47" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D15" t="s">
         <v>262</v>
@@ -6099,10 +6099,10 @@
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.2">
       <c r="C16" s="47" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D16" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="H16" s="47" t="s">
         <v>371</v>
@@ -6116,19 +6116,17 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C17" s="47" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D17" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="H17" s="47"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C18" s="47"/>
       <c r="H18" s="47"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C19" s="47"/>
       <c r="H19" s="47"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.2">
@@ -6218,6 +6216,7 @@
     <mergeCell ref="G3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6225,7 +6224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
EPBDS-7993 Fix for null values
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/String.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -19,14 +19,13 @@
     <sheet name="trim" sheetId="20" r:id="rId10"/>
     <sheet name="toString" sheetId="21" r:id="rId11"/>
     <sheet name="toNumbers" sheetId="22" r:id="rId12"/>
-    <sheet name="like" sheetId="26" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="255">
   <si>
     <t>return contains(str, searchChar);</t>
   </si>
@@ -791,144 +790,6 @@
   </si>
   <si>
     <t>0001.10000</t>
-  </si>
-  <si>
-    <t>_description_</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>pattern</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Method boolean likeMethod(String str, String pattern)</t>
-  </si>
-  <si>
-    <t>return like(str, pattern);</t>
-  </si>
-  <si>
-    <t>Test likeMethod</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>FFF</t>
-  </si>
-  <si>
-    <t>[!A-Z]</t>
-  </si>
-  <si>
-    <t>aTa</t>
-  </si>
-  <si>
-    <t>a#a</t>
-  </si>
-  <si>
-    <t>CAT123khg</t>
-  </si>
-  <si>
-    <t>B?T*</t>
-  </si>
-  <si>
-    <t>a2a</t>
-  </si>
-  <si>
-    <t>a@a</t>
-  </si>
-  <si>
-    <t>1E1234AE</t>
-  </si>
-  <si>
-    <t>@@####@@</t>
-  </si>
-  <si>
-    <t>A23-45AE</t>
-  </si>
-  <si>
-    <t>###-##@@</t>
-  </si>
-  <si>
-    <t>foo.bar@gmail.</t>
-  </si>
-  <si>
-    <t>foo.bar@gmailcom</t>
-  </si>
-  <si>
-    <t>+38(099)123-12-12</t>
-  </si>
-  <si>
-    <t>+7#(###)###-##-##</t>
-  </si>
-  <si>
-    <t>aBBBa</t>
-  </si>
-  <si>
-    <t>a*a</t>
-  </si>
-  <si>
-    <t>[A-Z]</t>
-  </si>
-  <si>
-    <t>BAR+</t>
-  </si>
-  <si>
-    <t>[A-Z]++</t>
-  </si>
-  <si>
-    <t>aM5b</t>
-  </si>
-  <si>
-    <t>a[L-P]#[!c-e]</t>
-  </si>
-  <si>
-    <t>BAT123khg</t>
-  </si>
-  <si>
-    <t>AE1234AE</t>
-  </si>
-  <si>
-    <t>123-45AE</t>
-  </si>
-  <si>
-    <t>###-##??+</t>
-  </si>
-  <si>
-    <t>123-45AE123</t>
-  </si>
-  <si>
-    <t>123-45-AE</t>
-  </si>
-  <si>
-    <t>#+-#+-@+</t>
-  </si>
-  <si>
-    <t>foo.bar@gmail.com</t>
-  </si>
-  <si>
-    <t>foo@bar.com</t>
-  </si>
-  <si>
-    <t>+38(099) 123-12-12</t>
-  </si>
-  <si>
-    <t>+##(###) ###-##-##</t>
-  </si>
-  <si>
-    <t>?+\@?+.?+</t>
-  </si>
-  <si>
-    <t>*\@*.*</t>
   </si>
 </sst>
 </file>
@@ -1232,9 +1093,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1251,6 +1109,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,29 +1503,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="B3" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1903,25 +1764,25 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="60"/>
-      <c r="D37" s="61"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="60"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -2089,7 +1950,7 @@
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f ca="1">TODAY()</f>
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>181</v>
@@ -2194,25 +2055,25 @@
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="62" t="s">
+      <c r="B69" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="63"/>
-      <c r="D69" s="63"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="64" t="s">
+      <c r="B70" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="63"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="C72" s="60"/>
-      <c r="D72" s="61"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="60"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="5" t="s">
@@ -2429,25 +2290,25 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="62" t="s">
+      <c r="B99" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="C99" s="62"/>
-      <c r="D99" s="62"/>
+      <c r="C99" s="61"/>
+      <c r="D99" s="61"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="58" t="s">
+      <c r="B100" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C100" s="58"/>
-      <c r="D100" s="58"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="59" t="s">
+      <c r="B102" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="C102" s="60"/>
-      <c r="D102" s="61"/>
+      <c r="C102" s="59"/>
+      <c r="D102" s="60"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="5" t="s">
@@ -2676,11 +2537,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B100:D100"/>
     <mergeCell ref="B102:D102"/>
     <mergeCell ref="B37:D37"/>
@@ -2688,6 +2544,11 @@
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2708,16 +2569,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="65" t="s">
@@ -2849,19 +2710,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="58" t="s">
         <v>240</v>
       </c>
       <c r="C6" s="67"/>
@@ -2960,7 +2821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -2971,31 +2832,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="61" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="E3" s="62" t="s">
+      <c r="C3" s="61"/>
+      <c r="E3" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="62"/>
+      <c r="F3" s="61"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="E4" s="58" t="s">
+      <c r="C4" s="64"/>
+      <c r="E4" s="64" t="s">
         <v>249</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="64"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="58" t="s">
         <v>244</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="58" t="s">
         <v>250</v>
       </c>
       <c r="F7" s="67"/>
@@ -3109,490 +2970,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E62"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="66" t="s">
-        <v>261</v>
-      </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="66" t="s">
-        <v>262</v>
-      </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>259</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>256</v>
-      </c>
-      <c r="C10" t="s">
-        <v>257</v>
-      </c>
-      <c r="D10" t="s">
-        <v>260</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C12" s="47"/>
-      <c r="D12" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="E12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C13" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="E13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C14" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>265</v>
-      </c>
-      <c r="E14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C15" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="E15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C16" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="E16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C17" s="47" t="s">
-        <v>269</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>270</v>
-      </c>
-      <c r="E17" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C18" s="47" t="s">
-        <v>271</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="E18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C19" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C20" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C21" s="47" t="s">
-        <v>277</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E21" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C22" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E22" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C23" s="47" t="s">
-        <v>279</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="E23" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C24" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="E24" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C25" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="E25" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C26" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>283</v>
-      </c>
-      <c r="E26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C27" s="47" t="s">
-        <v>284</v>
-      </c>
-      <c r="D27" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="E27" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="47" t="s">
-        <v>271</v>
-      </c>
-      <c r="D28" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="E28" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C29" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="E29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C30" s="47" t="s">
-        <v>286</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="E30" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C31" s="47" t="s">
-        <v>288</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>270</v>
-      </c>
-      <c r="E31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C32" s="47" t="s">
-        <v>289</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C33" s="47" t="s">
-        <v>290</v>
-      </c>
-      <c r="D33" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E33" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C34" s="47" t="s">
-        <v>290</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E34" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C35" s="47" t="s">
-        <v>290</v>
-      </c>
-      <c r="D35" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="E35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C36" s="47" t="s">
-        <v>292</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="E36" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C37" s="47" t="s">
-        <v>293</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>294</v>
-      </c>
-      <c r="E37" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C38" s="47" t="s">
-        <v>295</v>
-      </c>
-      <c r="D38" s="47" t="s">
-        <v>300</v>
-      </c>
-      <c r="E38" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C39" s="47" t="s">
-        <v>296</v>
-      </c>
-      <c r="D39" s="47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E39" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C40" s="47" t="s">
-        <v>297</v>
-      </c>
-      <c r="D40" s="47" t="s">
-        <v>298</v>
-      </c>
-      <c r="E40" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="47"/>
-      <c r="D54" s="47"/>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3613,25 +2990,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3870,25 +3247,25 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="61"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
@@ -4050,16 +3427,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="65" t="s">
@@ -4164,7 +3541,7 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f ca="1">TODAY()</f>
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="C18" s="18" t="b">
         <v>0</v>
@@ -4212,16 +3589,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="65" t="s">
@@ -4286,16 +3663,16 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="61"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="64"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="65" t="s">
@@ -4389,25 +3766,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4558,25 +3935,25 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="61"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
@@ -4722,28 +4099,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4975,31 +4352,31 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="61"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="60"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
@@ -5184,25 +4561,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="60"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -5291,28 +4668,28 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="60"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="41" t="s">
@@ -5640,16 +5017,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="64"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="65" t="s">

</xml_diff>